<commit_message>
fixed csv column headings
</commit_message>
<xml_diff>
--- a/data/dot_plot_merge_stacked_bar.xlsx
+++ b/data/dot_plot_merge_stacked_bar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajayrao/Desktop/DS4200_Sites/project-group-6-neuronal-regeneration/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AC76B2-6EE5-9042-A7D5-54E9172ED411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2AE86E-B323-8647-B48C-B07F6314499F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35800" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="63">
   <si>
     <t>﻿date</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>24hr_YA</t>
+  </si>
+  <si>
+    <t>re_image_time_class</t>
   </si>
 </sst>
 </file>
@@ -1050,10 +1053,14 @@
   <dimension ref="A1:P138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="J17" sqref="J17:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1084,7 +1091,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="K1" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
experimented with css styling and with linkinng styling
</commit_message>
<xml_diff>
--- a/data/dot_plot_merge_stacked_bar.xlsx
+++ b/data/dot_plot_merge_stacked_bar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augus\Documents\Northeastern\ds 4200 2\hw\project-group-6-neuronal-regeneration\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajayrao/Desktop/DS4200_Sites/project-group-6-neuronal-regeneration/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F32CBD-1F6A-4C4C-82C2-9CF03888F3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6C9A3B-341C-F24C-952D-F215763C211A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="938" yWindow="-98" windowWidth="23160" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36440" yWindow="1940" windowWidth="29000" windowHeight="18480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dot_plot_merge_stacked_bar" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="67">
   <si>
     <t>﻿date</t>
   </si>
@@ -1072,21 +1072,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T138"/>
+  <dimension ref="A1:T127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="7" max="9" width="10.83203125"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.9375" customWidth="1"/>
-    <col min="19" max="19" width="16.6875" customWidth="1"/>
+    <col min="18" max="18" width="17" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42212</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42212</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42212</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42212</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>42212</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>42212</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>42212</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>42219</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>42219</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>42219</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>42219</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>42219</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>42219</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>42219</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>42219</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>42213</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>42213</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>42213</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>42213</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>42213</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>42213</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>42213</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>42213</v>
       </c>
@@ -2127,15 +2127,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>42213</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
+      </c>
+      <c r="D25">
+        <v>41.825000000000003</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
@@ -2150,18 +2156,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>42213</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D26">
-        <v>41.825000000000003</v>
+        <v>61.02</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -2179,15 +2185,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>42213</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <v>62.475999999999999</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
       </c>
       <c r="F27" t="s">
         <v>11</v>
@@ -2202,18 +2214,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>42213</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28">
-        <v>61.02</v>
+        <v>34.966999999999999</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -2231,18 +2243,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>42213</v>
+        <v>42216</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D29">
-        <v>62.475999999999999</v>
+        <v>52.987000000000002</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -2260,18 +2272,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>42213</v>
+        <v>42216</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30">
-        <v>34.966999999999999</v>
+        <v>76.769000000000005</v>
       </c>
       <c r="E30">
         <v>3</v>
@@ -2289,21 +2301,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>42216</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D31">
-        <v>52.987000000000002</v>
+        <v>43.268999999999998</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F31" t="s">
         <v>11</v>
@@ -2318,15 +2330,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>42216</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="D32">
+        <v>18.236999999999998</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
       </c>
       <c r="F32" t="s">
         <v>11</v>
@@ -2341,21 +2359,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>42216</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
       </c>
       <c r="D33">
-        <v>76.769000000000005</v>
+        <v>74.686999999999998</v>
       </c>
       <c r="E33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F33" t="s">
         <v>11</v>
@@ -2370,18 +2388,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>42216</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
       </c>
       <c r="D34">
-        <v>43.268999999999998</v>
+        <v>50.05</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -2399,18 +2417,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>42216</v>
+        <v>42219</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D35">
-        <v>18.236999999999998</v>
+        <v>12.617000000000001</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -2419,88 +2437,88 @@
         <v>11</v>
       </c>
       <c r="G35" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>42216</v>
+        <v>42219</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D36">
-        <v>74.686999999999998</v>
+        <v>21.196000000000002</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F36" t="s">
         <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I36" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>42216</v>
+        <v>42219</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D37">
-        <v>50.05</v>
+        <v>32.209000000000003</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="s">
         <v>11</v>
       </c>
       <c r="G37" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>42219</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D38">
-        <v>12.617000000000001</v>
+        <v>50.768999999999998</v>
       </c>
       <c r="E38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F38" t="s">
         <v>11</v>
@@ -2515,21 +2533,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>42219</v>
+        <v>42221</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
       </c>
       <c r="D39">
-        <v>21.196000000000002</v>
+        <v>56.04</v>
       </c>
       <c r="E39">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F39" t="s">
         <v>11</v>
@@ -2544,21 +2562,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>42219</v>
+        <v>42221</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
         <v>10</v>
       </c>
       <c r="D40">
-        <v>32.209000000000003</v>
+        <v>44.686</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F40" t="s">
         <v>11</v>
@@ -2573,21 +2591,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>42219</v>
+        <v>42221</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D41">
-        <v>50.768999999999998</v>
+        <v>41.225000000000001</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="s">
         <v>11</v>
@@ -2602,21 +2620,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>42221</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D42">
-        <v>56.04</v>
+        <v>24.587</v>
       </c>
       <c r="E42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="s">
         <v>11</v>
@@ -2631,21 +2649,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42221</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
       </c>
       <c r="D43">
-        <v>44.686</v>
+        <v>63.823999999999998</v>
       </c>
       <c r="E43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="s">
         <v>11</v>
@@ -2660,21 +2678,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42221</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
       </c>
       <c r="D44">
-        <v>41.225000000000001</v>
+        <v>37.356000000000002</v>
       </c>
       <c r="E44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F44" t="s">
         <v>11</v>
@@ -2689,18 +2707,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>42221</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D45">
-        <v>24.587</v>
+        <v>57.383000000000003</v>
       </c>
       <c r="E45">
         <v>3</v>
@@ -2718,15 +2736,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>42221</v>
       </c>
       <c r="B46" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="D46">
+        <v>63.572000000000003</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
       </c>
       <c r="F46" t="s">
         <v>11</v>
@@ -2741,21 +2765,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>42221</v>
       </c>
       <c r="B47" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D47">
-        <v>63.823999999999998</v>
+        <v>57.125999999999998</v>
       </c>
       <c r="E47">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F47" t="s">
         <v>11</v>
@@ -2770,18 +2794,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>42221</v>
+        <v>42216</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C48" t="s">
         <v>10</v>
       </c>
       <c r="D48">
-        <v>37.356000000000002</v>
+        <v>53.774000000000001</v>
       </c>
       <c r="E48">
         <v>4</v>
@@ -2790,7 +2814,7 @@
         <v>11</v>
       </c>
       <c r="G48" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H48" t="s">
         <v>28</v>
@@ -2799,27 +2823,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>42221</v>
+        <v>42216</v>
       </c>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C49" t="s">
         <v>10</v>
       </c>
       <c r="D49">
-        <v>57.383000000000003</v>
+        <v>73.561000000000007</v>
       </c>
       <c r="E49">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F49" t="s">
         <v>11</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H49" t="s">
         <v>28</v>
@@ -2828,18 +2852,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>42221</v>
+        <v>42216</v>
       </c>
       <c r="B50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D50">
-        <v>63.572000000000003</v>
+        <v>66.263000000000005</v>
       </c>
       <c r="E50">
         <v>4</v>
@@ -2848,7 +2872,7 @@
         <v>11</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H50" t="s">
         <v>28</v>
@@ -2857,9 +2881,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>42221</v>
+        <v>42216</v>
       </c>
       <c r="B51" t="s">
         <v>34</v>
@@ -2868,7 +2892,7 @@
         <v>18</v>
       </c>
       <c r="D51">
-        <v>57.125999999999998</v>
+        <v>86.914000000000001</v>
       </c>
       <c r="E51">
         <v>4</v>
@@ -2877,7 +2901,7 @@
         <v>11</v>
       </c>
       <c r="G51" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H51" t="s">
         <v>28</v>
@@ -2886,18 +2910,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>42216</v>
+        <v>42220</v>
       </c>
       <c r="B52" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
       </c>
       <c r="D52">
-        <v>53.774000000000001</v>
+        <v>55.014000000000003</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -2915,18 +2939,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>42216</v>
+        <v>42220</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C53" t="s">
         <v>10</v>
       </c>
       <c r="D53">
-        <v>73.561000000000007</v>
+        <v>64.063999999999993</v>
       </c>
       <c r="E53">
         <v>4</v>
@@ -2944,18 +2968,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>42216</v>
+        <v>42220</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D54">
-        <v>66.263000000000005</v>
+        <v>55.926000000000002</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -2973,16 +2997,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>42216</v>
+        <v>42222</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C55" t="s">
         <v>10</v>
       </c>
+      <c r="D55">
+        <v>46.652000000000001</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
       <c r="F55" t="s">
         <v>11</v>
       </c>
@@ -2996,15 +3026,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>42216</v>
+        <v>42222</v>
       </c>
       <c r="B56" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C56" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D56">
+        <v>89.188000000000002</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
       </c>
       <c r="F56" t="s">
         <v>11</v>
@@ -3019,18 +3055,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>42216</v>
+        <v>42222</v>
       </c>
       <c r="B57" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D57">
-        <v>86.914000000000001</v>
+        <v>99.19</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -3048,15 +3084,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>42216</v>
+        <v>42222</v>
       </c>
       <c r="B58" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D58">
+        <v>48.997999999999998</v>
+      </c>
+      <c r="E58">
+        <v>4</v>
       </c>
       <c r="F58" t="s">
         <v>11</v>
@@ -3071,18 +3113,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>42220</v>
+        <v>42222</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D59">
-        <v>55.014000000000003</v>
+        <v>99.488</v>
       </c>
       <c r="E59">
         <v>4</v>
@@ -3100,15 +3142,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>42220</v>
+        <v>42222</v>
       </c>
       <c r="B60" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="D60">
+        <v>90.728999999999999</v>
+      </c>
+      <c r="E60">
+        <v>4</v>
       </c>
       <c r="F60" t="s">
         <v>11</v>
@@ -3123,18 +3171,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>42220</v>
+        <v>42222</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D61">
-        <v>64.063999999999993</v>
+        <v>67.787000000000006</v>
       </c>
       <c r="E61">
         <v>4</v>
@@ -3152,18 +3200,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>42220</v>
+        <v>42222</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C62" t="s">
         <v>18</v>
       </c>
       <c r="D62">
-        <v>55.926000000000002</v>
+        <v>51.698</v>
       </c>
       <c r="E62">
         <v>4</v>
@@ -3181,313 +3229,331 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>42222</v>
+        <v>42213</v>
       </c>
       <c r="B63" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C63" t="s">
         <v>10</v>
       </c>
       <c r="D63">
-        <v>46.652000000000001</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F63" t="s">
         <v>11</v>
       </c>
       <c r="G63" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H63" t="s">
         <v>28</v>
       </c>
       <c r="I63" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>42222</v>
+        <v>42213</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D64">
-        <v>89.188000000000002</v>
+        <v>0</v>
       </c>
       <c r="E64">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F64" t="s">
         <v>11</v>
       </c>
       <c r="G64" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H64" t="s">
         <v>28</v>
       </c>
       <c r="I64" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>42222</v>
+        <v>42213</v>
       </c>
       <c r="B65" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C65" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
       </c>
       <c r="F65" t="s">
         <v>11</v>
       </c>
       <c r="G65" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H65" t="s">
         <v>28</v>
       </c>
       <c r="I65" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>42222</v>
+        <v>42213</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
       </c>
       <c r="F66" t="s">
         <v>11</v>
       </c>
       <c r="G66" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H66" t="s">
         <v>28</v>
       </c>
       <c r="I66" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>42222</v>
+        <v>42213</v>
       </c>
       <c r="B67" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C67" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D67">
-        <v>99.19</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F67" t="s">
         <v>11</v>
       </c>
       <c r="G67" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H67" t="s">
         <v>28</v>
       </c>
       <c r="I67" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>42222</v>
+        <v>42213</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C68" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D68">
-        <v>48.997999999999998</v>
+        <v>0</v>
       </c>
       <c r="E68">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F68" t="s">
         <v>11</v>
       </c>
       <c r="G68" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H68" t="s">
         <v>28</v>
       </c>
       <c r="I68" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>42222</v>
+        <v>42213</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C69" t="s">
         <v>18</v>
       </c>
       <c r="D69">
-        <v>99.488</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F69" t="s">
         <v>11</v>
       </c>
       <c r="G69" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H69" t="s">
         <v>28</v>
       </c>
       <c r="I69" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>42222</v>
+        <v>42213</v>
       </c>
       <c r="B70" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C70" t="s">
         <v>18</v>
       </c>
       <c r="D70">
-        <v>90.728999999999999</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F70" t="s">
         <v>11</v>
       </c>
       <c r="G70" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H70" t="s">
         <v>28</v>
       </c>
       <c r="I70" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>42222</v>
+        <v>42213</v>
       </c>
       <c r="B71" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C71" t="s">
         <v>18</v>
       </c>
       <c r="D71">
-        <v>67.787000000000006</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F71" t="s">
         <v>11</v>
       </c>
       <c r="G71" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H71" t="s">
         <v>28</v>
       </c>
       <c r="I71" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>42222</v>
+        <v>42216</v>
       </c>
       <c r="B72" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C72" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D72">
-        <v>51.698</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F72" t="s">
         <v>11</v>
       </c>
       <c r="G72" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H72" t="s">
         <v>28</v>
       </c>
       <c r="I72" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>42222</v>
+        <v>42216</v>
       </c>
       <c r="B73" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D73">
+        <v>3.9830000000000001</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
       </c>
       <c r="F73" t="s">
         <v>11</v>
       </c>
       <c r="G73" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H73" t="s">
         <v>28</v>
       </c>
       <c r="I73" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>42213</v>
+        <v>42216</v>
       </c>
       <c r="B74" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C74" t="s">
         <v>10</v>
@@ -3511,15 +3577,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>42213</v>
+        <v>42216</v>
       </c>
       <c r="B75" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C75" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -3540,12 +3606,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>42213</v>
+        <v>42216</v>
       </c>
       <c r="B76" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C76" t="s">
         <v>18</v>
@@ -3569,12 +3635,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>42213</v>
+        <v>42216</v>
       </c>
       <c r="B77" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C77" t="s">
         <v>18</v>
@@ -3598,27 +3664,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>42213</v>
+        <v>42214</v>
       </c>
       <c r="B78" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C78" t="s">
         <v>18</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>38.116</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F78" t="s">
         <v>11</v>
       </c>
       <c r="G78" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H78" t="s">
         <v>28</v>
@@ -3627,27 +3693,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>42213</v>
+        <v>42214</v>
       </c>
       <c r="B79" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C79" t="s">
         <v>18</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>4.3650000000000002</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" t="s">
         <v>11</v>
       </c>
       <c r="G79" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H79" t="s">
         <v>28</v>
@@ -3656,12 +3722,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>42213</v>
+        <v>42214</v>
       </c>
       <c r="B80" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C80" t="s">
         <v>18</v>
@@ -3676,7 +3742,7 @@
         <v>11</v>
       </c>
       <c r="G80" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H80" t="s">
         <v>28</v>
@@ -3685,27 +3751,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>42213</v>
+        <v>42214</v>
       </c>
       <c r="B81" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C81" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>7.5629999999999997</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" t="s">
         <v>11</v>
       </c>
       <c r="G81" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H81" t="s">
         <v>28</v>
@@ -3714,27 +3780,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>42213</v>
+        <v>42214</v>
       </c>
       <c r="B82" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C82" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>22.725999999999999</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F82" t="s">
         <v>11</v>
       </c>
       <c r="G82" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H82" t="s">
         <v>28</v>
@@ -3743,27 +3809,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>42216</v>
+        <v>42214</v>
       </c>
       <c r="B83" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C83" t="s">
         <v>10</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>7.3220000000000001</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" t="s">
         <v>11</v>
       </c>
       <c r="G83" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H83" t="s">
         <v>28</v>
@@ -3772,27 +3838,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>42216</v>
+        <v>42214</v>
       </c>
       <c r="B84" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C84" t="s">
         <v>10</v>
       </c>
       <c r="D84">
-        <v>3.9830000000000001</v>
+        <v>19.681999999999999</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F84" t="s">
         <v>11</v>
       </c>
       <c r="G84" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H84" t="s">
         <v>28</v>
@@ -3801,12 +3867,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>42216</v>
+        <v>42214</v>
       </c>
       <c r="B85" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C85" t="s">
         <v>10</v>
@@ -3821,7 +3887,7 @@
         <v>11</v>
       </c>
       <c r="G85" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H85" t="s">
         <v>28</v>
@@ -3830,27 +3896,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>42216</v>
       </c>
       <c r="B86" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C86" t="s">
         <v>10</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>5.6189999999999998</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" t="s">
         <v>11</v>
       </c>
       <c r="G86" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H86" t="s">
         <v>28</v>
@@ -3859,15 +3925,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>42216</v>
       </c>
       <c r="B87" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C87" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -3879,7 +3945,7 @@
         <v>11</v>
       </c>
       <c r="G87" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H87" t="s">
         <v>28</v>
@@ -3888,15 +3954,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>42216</v>
       </c>
       <c r="B88" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C88" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -3908,7 +3974,7 @@
         <v>11</v>
       </c>
       <c r="G88" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H88" t="s">
         <v>28</v>
@@ -3917,21 +3983,21 @@
         <v>48</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>42214</v>
+        <v>42216</v>
       </c>
       <c r="B89" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C89" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D89">
-        <v>38.116</v>
+        <v>0</v>
       </c>
       <c r="E89">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F89" t="s">
         <v>11</v>
@@ -3946,21 +4012,21 @@
         <v>48</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>42214</v>
+        <v>42216</v>
       </c>
       <c r="B90" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C90" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D90">
-        <v>4.3650000000000002</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90" t="s">
         <v>11</v>
@@ -3975,21 +4041,21 @@
         <v>48</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>42214</v>
+        <v>42216</v>
       </c>
       <c r="B91" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C91" t="s">
         <v>18</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>24.18</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F91" t="s">
         <v>11</v>
@@ -4004,18 +4070,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>42214</v>
+        <v>42216</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C92" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D92">
-        <v>7.5629999999999997</v>
+        <v>5.1120000000000001</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -4033,21 +4099,21 @@
         <v>48</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>42214</v>
+        <v>42216</v>
       </c>
       <c r="B93" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C93" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D93">
-        <v>22.725999999999999</v>
+        <v>22.388999999999999</v>
       </c>
       <c r="E93">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="s">
         <v>11</v>
@@ -4062,340 +4128,340 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>42214</v>
+        <v>42250</v>
       </c>
       <c r="B94" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C94" t="s">
         <v>10</v>
       </c>
       <c r="D94">
-        <v>7.3220000000000001</v>
+        <v>27.48</v>
       </c>
       <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94" t="s">
+        <v>49</v>
+      </c>
+      <c r="G94" t="s">
+        <v>25</v>
+      </c>
+      <c r="H94" t="s">
+        <v>13</v>
+      </c>
+      <c r="I94" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>42250</v>
+      </c>
+      <c r="B95" t="s">
+        <v>24</v>
+      </c>
+      <c r="C95" t="s">
+        <v>10</v>
+      </c>
+      <c r="D95">
+        <v>16.446999999999999</v>
+      </c>
+      <c r="E95">
         <v>1</v>
       </c>
-      <c r="F94" t="s">
-        <v>11</v>
-      </c>
-      <c r="G94" t="s">
-        <v>25</v>
-      </c>
-      <c r="H94" t="s">
-        <v>28</v>
-      </c>
-      <c r="I94" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A95" s="1">
-        <v>42214</v>
-      </c>
-      <c r="B95" t="s">
-        <v>17</v>
-      </c>
-      <c r="C95" t="s">
-        <v>10</v>
-      </c>
-      <c r="D95">
-        <v>19.681999999999999</v>
-      </c>
-      <c r="E95">
+      <c r="F95" t="s">
+        <v>49</v>
+      </c>
+      <c r="G95" t="s">
+        <v>25</v>
+      </c>
+      <c r="H95" t="s">
+        <v>13</v>
+      </c>
+      <c r="I95" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>42250</v>
+      </c>
+      <c r="B96" t="s">
+        <v>20</v>
+      </c>
+      <c r="C96" t="s">
+        <v>18</v>
+      </c>
+      <c r="D96">
+        <v>13.541</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96" t="s">
+        <v>49</v>
+      </c>
+      <c r="G96" t="s">
+        <v>25</v>
+      </c>
+      <c r="H96" t="s">
+        <v>13</v>
+      </c>
+      <c r="I96" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B97" t="s">
+        <v>22</v>
+      </c>
+      <c r="C97" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97">
+        <v>72.948999999999998</v>
+      </c>
+      <c r="E97">
+        <v>3</v>
+      </c>
+      <c r="F97" t="s">
+        <v>49</v>
+      </c>
+      <c r="G97" t="s">
+        <v>25</v>
+      </c>
+      <c r="H97" t="s">
+        <v>13</v>
+      </c>
+      <c r="I97" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B98" t="s">
+        <v>23</v>
+      </c>
+      <c r="C98" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98">
+        <v>43.543999999999997</v>
+      </c>
+      <c r="E98">
         <v>2</v>
       </c>
-      <c r="F95" t="s">
-        <v>11</v>
-      </c>
-      <c r="G95" t="s">
-        <v>25</v>
-      </c>
-      <c r="H95" t="s">
-        <v>28</v>
-      </c>
-      <c r="I95" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A96" s="1">
-        <v>42214</v>
-      </c>
-      <c r="B96" t="s">
-        <v>19</v>
-      </c>
-      <c r="C96" t="s">
-        <v>10</v>
-      </c>
-      <c r="D96">
-        <v>0</v>
-      </c>
-      <c r="E96">
-        <v>0</v>
-      </c>
-      <c r="F96" t="s">
-        <v>11</v>
-      </c>
-      <c r="G96" t="s">
-        <v>25</v>
-      </c>
-      <c r="H96" t="s">
-        <v>28</v>
-      </c>
-      <c r="I96" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A97" s="1">
-        <v>42216</v>
-      </c>
-      <c r="B97" t="s">
-        <v>37</v>
-      </c>
-      <c r="C97" t="s">
-        <v>10</v>
-      </c>
-      <c r="D97">
-        <v>5.6189999999999998</v>
-      </c>
-      <c r="E97">
+      <c r="F98" t="s">
+        <v>49</v>
+      </c>
+      <c r="G98" t="s">
+        <v>25</v>
+      </c>
+      <c r="H98" t="s">
+        <v>13</v>
+      </c>
+      <c r="I98" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C99" t="s">
+        <v>18</v>
+      </c>
+      <c r="D99">
+        <v>54.895000000000003</v>
+      </c>
+      <c r="E99">
+        <v>3</v>
+      </c>
+      <c r="F99" t="s">
+        <v>49</v>
+      </c>
+      <c r="G99" t="s">
+        <v>25</v>
+      </c>
+      <c r="H99" t="s">
+        <v>13</v>
+      </c>
+      <c r="I99" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B100" t="s">
+        <v>36</v>
+      </c>
+      <c r="C100" t="s">
+        <v>18</v>
+      </c>
+      <c r="D100">
+        <v>9.641</v>
+      </c>
+      <c r="E100">
         <v>1</v>
       </c>
-      <c r="F97" t="s">
-        <v>11</v>
-      </c>
-      <c r="G97" t="s">
-        <v>25</v>
-      </c>
-      <c r="H97" t="s">
-        <v>28</v>
-      </c>
-      <c r="I97" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A98" s="1">
-        <v>42216</v>
-      </c>
-      <c r="B98" t="s">
-        <v>38</v>
-      </c>
-      <c r="C98" t="s">
-        <v>10</v>
-      </c>
-      <c r="D98">
-        <v>0</v>
-      </c>
-      <c r="E98">
-        <v>0</v>
-      </c>
-      <c r="F98" t="s">
-        <v>11</v>
-      </c>
-      <c r="G98" t="s">
-        <v>25</v>
-      </c>
-      <c r="H98" t="s">
-        <v>28</v>
-      </c>
-      <c r="I98" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A99" s="1">
-        <v>42216</v>
-      </c>
-      <c r="B99" t="s">
-        <v>39</v>
-      </c>
-      <c r="C99" t="s">
-        <v>10</v>
-      </c>
-      <c r="D99">
-        <v>0</v>
-      </c>
-      <c r="E99">
-        <v>0</v>
-      </c>
-      <c r="F99" t="s">
-        <v>11</v>
-      </c>
-      <c r="G99" t="s">
-        <v>25</v>
-      </c>
-      <c r="H99" t="s">
-        <v>28</v>
-      </c>
-      <c r="I99" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A100" s="1">
-        <v>42216</v>
-      </c>
-      <c r="B100" t="s">
-        <v>40</v>
-      </c>
-      <c r="C100" t="s">
-        <v>10</v>
-      </c>
-      <c r="D100">
-        <v>0</v>
-      </c>
-      <c r="E100">
-        <v>0</v>
-      </c>
       <c r="F100" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="G100" t="s">
         <v>25</v>
       </c>
       <c r="H100" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I100" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>42216</v>
+        <v>42258</v>
       </c>
       <c r="B101" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C101" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>9.42</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="G101" t="s">
         <v>25</v>
       </c>
       <c r="H101" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I101" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>42216</v>
+        <v>42258</v>
       </c>
       <c r="B102" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C102" t="s">
         <v>18</v>
       </c>
       <c r="D102">
-        <v>24.18</v>
+        <v>47.5</v>
       </c>
       <c r="E102">
         <v>3</v>
       </c>
       <c r="F102" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="G102" t="s">
         <v>25</v>
       </c>
       <c r="H102" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I102" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>42216</v>
+        <v>42258</v>
       </c>
       <c r="B103" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C103" t="s">
         <v>18</v>
       </c>
       <c r="D103">
-        <v>5.1120000000000001</v>
+        <v>14.042</v>
       </c>
       <c r="E103">
         <v>1</v>
       </c>
       <c r="F103" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="G103" t="s">
         <v>25</v>
       </c>
       <c r="H103" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I103" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>42216</v>
+        <v>42258</v>
       </c>
       <c r="B104" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C104" t="s">
         <v>18</v>
       </c>
       <c r="D104">
-        <v>22.388999999999999</v>
+        <v>18.603000000000002</v>
       </c>
       <c r="E104">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F104" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="G104" t="s">
         <v>25</v>
       </c>
       <c r="H104" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I104" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>42250</v>
+        <v>42258</v>
       </c>
       <c r="B105" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C105" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D105">
-        <v>27.48</v>
+        <v>3.9140000000000001</v>
       </c>
       <c r="E105">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F105" t="s">
         <v>49</v>
@@ -4410,21 +4476,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>42250</v>
       </c>
       <c r="B106" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C106" t="s">
         <v>10</v>
       </c>
       <c r="D106">
-        <v>16.446999999999999</v>
+        <v>65.301000000000002</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F106" t="s">
         <v>49</v>
@@ -4433,27 +4499,27 @@
         <v>25</v>
       </c>
       <c r="H106" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I106" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>42250</v>
       </c>
       <c r="B107" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D107">
-        <v>13.541</v>
+        <v>71.745999999999995</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F107" t="s">
         <v>49</v>
@@ -4462,24 +4528,24 @@
         <v>25</v>
       </c>
       <c r="H107" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I107" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>42258</v>
+        <v>42250</v>
       </c>
       <c r="B108" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C108" t="s">
         <v>10</v>
       </c>
       <c r="D108">
-        <v>72.948999999999998</v>
+        <v>80.382000000000005</v>
       </c>
       <c r="E108">
         <v>3</v>
@@ -4491,27 +4557,27 @@
         <v>25</v>
       </c>
       <c r="H108" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I108" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>42258</v>
+        <v>42250</v>
       </c>
       <c r="B109" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C109" t="s">
         <v>18</v>
       </c>
       <c r="D109">
-        <v>43.543999999999997</v>
+        <v>55.499000000000002</v>
       </c>
       <c r="E109">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F109" t="s">
         <v>49</v>
@@ -4520,24 +4586,24 @@
         <v>25</v>
       </c>
       <c r="H109" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I109" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>42258</v>
+        <v>42250</v>
       </c>
       <c r="B110" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C110" t="s">
         <v>18</v>
       </c>
       <c r="D110">
-        <v>54.895000000000003</v>
+        <v>70.284999999999997</v>
       </c>
       <c r="E110">
         <v>3</v>
@@ -4549,27 +4615,27 @@
         <v>25</v>
       </c>
       <c r="H110" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I110" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>42258</v>
       </c>
       <c r="B111" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C111" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D111">
-        <v>9.641</v>
+        <v>78.337999999999994</v>
       </c>
       <c r="E111">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F111" t="s">
         <v>49</v>
@@ -4578,27 +4644,27 @@
         <v>25</v>
       </c>
       <c r="H111" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I111" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>42258</v>
       </c>
       <c r="B112" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C112" t="s">
         <v>18</v>
       </c>
       <c r="D112">
-        <v>9.42</v>
+        <v>67.725999999999999</v>
       </c>
       <c r="E112">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F112" t="s">
         <v>49</v>
@@ -4607,24 +4673,24 @@
         <v>25</v>
       </c>
       <c r="H112" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I112" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>42258</v>
       </c>
       <c r="B113" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C113" t="s">
         <v>18</v>
       </c>
       <c r="D113">
-        <v>47.5</v>
+        <v>63.298000000000002</v>
       </c>
       <c r="E113">
         <v>3</v>
@@ -4636,27 +4702,27 @@
         <v>25</v>
       </c>
       <c r="H113" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I113" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>42258</v>
       </c>
       <c r="B114" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C114" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D114">
-        <v>14.042</v>
+        <v>64.606999999999999</v>
       </c>
       <c r="E114">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F114" t="s">
         <v>49</v>
@@ -4665,24 +4731,24 @@
         <v>25</v>
       </c>
       <c r="H114" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I114" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>42258</v>
       </c>
       <c r="B115" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C115" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D115">
-        <v>18.603000000000002</v>
+        <v>89.617999999999995</v>
       </c>
       <c r="E115">
         <v>3</v>
@@ -4694,27 +4760,27 @@
         <v>25</v>
       </c>
       <c r="H115" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I115" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>42258</v>
       </c>
       <c r="B116" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C116" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D116">
-        <v>3.9140000000000001</v>
+        <v>95.587000000000003</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F116" t="s">
         <v>49</v>
@@ -4723,27 +4789,27 @@
         <v>25</v>
       </c>
       <c r="H116" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I116" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>42250</v>
+        <v>42258</v>
       </c>
       <c r="B117" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C117" t="s">
         <v>10</v>
       </c>
       <c r="D117">
-        <v>65.301000000000002</v>
+        <v>9.49</v>
       </c>
       <c r="E117">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F117" t="s">
         <v>49</v>
@@ -4755,24 +4821,24 @@
         <v>28</v>
       </c>
       <c r="I117" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>42250</v>
+        <v>42258</v>
       </c>
       <c r="B118" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C118" t="s">
         <v>10</v>
       </c>
       <c r="D118">
-        <v>71.745999999999995</v>
+        <v>4.1970000000000001</v>
       </c>
       <c r="E118">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F118" t="s">
         <v>49</v>
@@ -4784,24 +4850,24 @@
         <v>28</v>
       </c>
       <c r="I118" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>42250</v>
+        <v>42258</v>
       </c>
       <c r="B119" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C119" t="s">
         <v>10</v>
       </c>
       <c r="D119">
-        <v>80.382000000000005</v>
+        <v>0</v>
       </c>
       <c r="E119">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F119" t="s">
         <v>49</v>
@@ -4813,24 +4879,24 @@
         <v>28</v>
       </c>
       <c r="I119" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>42250</v>
+        <v>42258</v>
       </c>
       <c r="B120" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C120" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D120">
-        <v>55.499000000000002</v>
+        <v>12.788</v>
       </c>
       <c r="E120">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F120" t="s">
         <v>49</v>
@@ -4842,24 +4908,24 @@
         <v>28</v>
       </c>
       <c r="I120" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>42250</v>
+        <v>42258</v>
       </c>
       <c r="B121" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C121" t="s">
         <v>18</v>
       </c>
       <c r="D121">
-        <v>70.284999999999997</v>
+        <v>0</v>
       </c>
       <c r="E121">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F121" t="s">
         <v>49</v>
@@ -4871,24 +4937,24 @@
         <v>28</v>
       </c>
       <c r="I121" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>42258</v>
       </c>
       <c r="B122" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C122" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D122">
-        <v>78.337999999999994</v>
+        <v>12.565</v>
       </c>
       <c r="E122">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F122" t="s">
         <v>49</v>
@@ -4900,24 +4966,24 @@
         <v>28</v>
       </c>
       <c r="I122" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>42258</v>
       </c>
       <c r="B123" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C123" t="s">
         <v>18</v>
       </c>
       <c r="D123">
-        <v>67.725999999999999</v>
+        <v>10.692</v>
       </c>
       <c r="E123">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F123" t="s">
         <v>49</v>
@@ -4929,24 +4995,24 @@
         <v>28</v>
       </c>
       <c r="I123" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>42258</v>
       </c>
       <c r="B124" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C124" t="s">
         <v>18</v>
       </c>
       <c r="D124">
-        <v>63.298000000000002</v>
+        <v>2.145</v>
       </c>
       <c r="E124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F124" t="s">
         <v>49</v>
@@ -4958,24 +5024,24 @@
         <v>28</v>
       </c>
       <c r="I124" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>42258</v>
       </c>
       <c r="B125" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C125" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D125">
-        <v>64.606999999999999</v>
+        <v>2.1850000000000001</v>
       </c>
       <c r="E125">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F125" t="s">
         <v>49</v>
@@ -4987,24 +5053,24 @@
         <v>28</v>
       </c>
       <c r="I125" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>42258</v>
       </c>
       <c r="B126" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C126" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D126">
-        <v>89.617999999999995</v>
+        <v>12.779</v>
       </c>
       <c r="E126">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F126" t="s">
         <v>49</v>
@@ -5016,24 +5082,24 @@
         <v>28</v>
       </c>
       <c r="I126" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>42258</v>
       </c>
       <c r="B127" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C127" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D127">
-        <v>95.587000000000003</v>
+        <v>0</v>
       </c>
       <c r="E127">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F127" t="s">
         <v>49</v>
@@ -5045,325 +5111,6 @@
         <v>28</v>
       </c>
       <c r="I127" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A128" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B128" t="s">
-        <v>37</v>
-      </c>
-      <c r="C128" t="s">
-        <v>10</v>
-      </c>
-      <c r="D128">
-        <v>9.49</v>
-      </c>
-      <c r="E128">
-        <v>1</v>
-      </c>
-      <c r="F128" t="s">
-        <v>49</v>
-      </c>
-      <c r="G128" t="s">
-        <v>25</v>
-      </c>
-      <c r="H128" t="s">
-        <v>28</v>
-      </c>
-      <c r="I128" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A129" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B129" t="s">
-        <v>38</v>
-      </c>
-      <c r="C129" t="s">
-        <v>10</v>
-      </c>
-      <c r="D129">
-        <v>4.1970000000000001</v>
-      </c>
-      <c r="E129">
-        <v>1</v>
-      </c>
-      <c r="F129" t="s">
-        <v>49</v>
-      </c>
-      <c r="G129" t="s">
-        <v>25</v>
-      </c>
-      <c r="H129" t="s">
-        <v>28</v>
-      </c>
-      <c r="I129" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A130" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B130" t="s">
-        <v>39</v>
-      </c>
-      <c r="C130" t="s">
-        <v>10</v>
-      </c>
-      <c r="D130">
-        <v>0</v>
-      </c>
-      <c r="E130">
-        <v>0</v>
-      </c>
-      <c r="F130" t="s">
-        <v>49</v>
-      </c>
-      <c r="G130" t="s">
-        <v>25</v>
-      </c>
-      <c r="H130" t="s">
-        <v>28</v>
-      </c>
-      <c r="I130" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A131" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B131" t="s">
-        <v>40</v>
-      </c>
-      <c r="C131" t="s">
-        <v>10</v>
-      </c>
-      <c r="D131">
-        <v>12.788</v>
-      </c>
-      <c r="E131">
-        <v>1</v>
-      </c>
-      <c r="F131" t="s">
-        <v>49</v>
-      </c>
-      <c r="G131" t="s">
-        <v>25</v>
-      </c>
-      <c r="H131" t="s">
-        <v>28</v>
-      </c>
-      <c r="I131" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A132" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B132" t="s">
-        <v>42</v>
-      </c>
-      <c r="C132" t="s">
-        <v>18</v>
-      </c>
-      <c r="D132">
-        <v>0</v>
-      </c>
-      <c r="E132">
-        <v>0</v>
-      </c>
-      <c r="F132" t="s">
-        <v>49</v>
-      </c>
-      <c r="G132" t="s">
-        <v>25</v>
-      </c>
-      <c r="H132" t="s">
-        <v>28</v>
-      </c>
-      <c r="I132" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A133" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B133" t="s">
-        <v>43</v>
-      </c>
-      <c r="C133" t="s">
-        <v>18</v>
-      </c>
-      <c r="D133">
-        <v>12.565</v>
-      </c>
-      <c r="E133">
-        <v>1</v>
-      </c>
-      <c r="F133" t="s">
-        <v>49</v>
-      </c>
-      <c r="G133" t="s">
-        <v>25</v>
-      </c>
-      <c r="H133" t="s">
-        <v>28</v>
-      </c>
-      <c r="I133" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A134" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B134" t="s">
-        <v>44</v>
-      </c>
-      <c r="C134" t="s">
-        <v>18</v>
-      </c>
-      <c r="D134">
-        <v>10.692</v>
-      </c>
-      <c r="E134">
-        <v>1</v>
-      </c>
-      <c r="F134" t="s">
-        <v>49</v>
-      </c>
-      <c r="G134" t="s">
-        <v>25</v>
-      </c>
-      <c r="H134" t="s">
-        <v>28</v>
-      </c>
-      <c r="I134" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A135" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B135" t="s">
-        <v>45</v>
-      </c>
-      <c r="C135" t="s">
-        <v>18</v>
-      </c>
-      <c r="D135">
-        <v>2.145</v>
-      </c>
-      <c r="E135">
-        <v>1</v>
-      </c>
-      <c r="F135" t="s">
-        <v>49</v>
-      </c>
-      <c r="G135" t="s">
-        <v>25</v>
-      </c>
-      <c r="H135" t="s">
-        <v>28</v>
-      </c>
-      <c r="I135" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A136" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B136" t="s">
-        <v>46</v>
-      </c>
-      <c r="C136" t="s">
-        <v>18</v>
-      </c>
-      <c r="D136">
-        <v>2.1850000000000001</v>
-      </c>
-      <c r="E136">
-        <v>1</v>
-      </c>
-      <c r="F136" t="s">
-        <v>49</v>
-      </c>
-      <c r="G136" t="s">
-        <v>25</v>
-      </c>
-      <c r="H136" t="s">
-        <v>28</v>
-      </c>
-      <c r="I136" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A137" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B137" t="s">
-        <v>47</v>
-      </c>
-      <c r="C137" t="s">
-        <v>18</v>
-      </c>
-      <c r="D137">
-        <v>12.779</v>
-      </c>
-      <c r="E137">
-        <v>1</v>
-      </c>
-      <c r="F137" t="s">
-        <v>49</v>
-      </c>
-      <c r="G137" t="s">
-        <v>25</v>
-      </c>
-      <c r="H137" t="s">
-        <v>28</v>
-      </c>
-      <c r="I137" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A138" s="1">
-        <v>42258</v>
-      </c>
-      <c r="B138" t="s">
-        <v>51</v>
-      </c>
-      <c r="C138" t="s">
-        <v>18</v>
-      </c>
-      <c r="D138">
-        <v>0</v>
-      </c>
-      <c r="E138">
-        <v>0</v>
-      </c>
-      <c r="F138" t="s">
-        <v>49</v>
-      </c>
-      <c r="G138" t="s">
-        <v>25</v>
-      </c>
-      <c r="H138" t="s">
-        <v>28</v>
-      </c>
-      <c r="I138" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>